<commit_message>
Completed Inserting Excel Shapes
</commit_message>
<xml_diff>
--- a/07 - Inserting Images and Shapes/MonthlyBudget.xlsx
+++ b/07 - Inserting Images and Shapes/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/07 - Inserting Images and Shapes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6081524E-D8D9-4C2A-AB68-781F6E4EE0FA}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFE9C84F-7B04-4F78-8099-5CD3758F5138}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -209,6 +209,131 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>68943</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>169636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>59872</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>17237</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Arrow: Left 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CE2DD91-0771-380D-7256-3B80699752C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7590972" y="1007836"/>
+          <a:ext cx="600529" cy="250372"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>160564</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>22679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>564243</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>428172</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Smiley Face 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7034D12-5DF2-CB8C-D662-C0E81F1E3169}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6740978" y="207736"/>
+          <a:ext cx="403679" cy="405493"/>
+        </a:xfrm>
+        <a:prstGeom prst="smileyFace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -835,5 +960,6 @@
   <ignoredErrors>
     <ignoredError sqref="C13:E16 C11:F11" formulaRange="1"/>
   </ignoredErrors>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Formatting Excel Shapes
</commit_message>
<xml_diff>
--- a/07 - Inserting Images and Shapes/MonthlyBudget.xlsx
+++ b/07 - Inserting Images and Shapes/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/07 - Inserting Images and Shapes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFE9C84F-7B04-4F78-8099-5CD3758F5138}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6218C0B-6658-4A33-B89D-64EF6CECB6B7}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,15 +216,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>68943</xdr:colOff>
+      <xdr:colOff>71664</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>169636</xdr:rowOff>
+      <xdr:rowOff>176892</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>59872</xdr:colOff>
+      <xdr:colOff>66221</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>17237</xdr:rowOff>
+      <xdr:rowOff>24493</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -239,12 +239,23 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7590972" y="1007836"/>
-          <a:ext cx="600529" cy="250372"/>
+          <a:off x="7593693" y="1015092"/>
+          <a:ext cx="604157" cy="250372"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 43479"/>
+            <a:gd name="adj2" fmla="val 97826"/>
+          </a:avLst>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -276,15 +287,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>160564</xdr:colOff>
+      <xdr:colOff>157843</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>22679</xdr:rowOff>
+      <xdr:rowOff>28121</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>564243</xdr:colOff>
+      <xdr:colOff>566964</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>428172</xdr:rowOff>
+      <xdr:rowOff>425451</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -299,12 +310,22 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6740978" y="207736"/>
-          <a:ext cx="403679" cy="405493"/>
+          <a:off x="6738257" y="213178"/>
+          <a:ext cx="409121" cy="397330"/>
         </a:xfrm>
         <a:prstGeom prst="smileyFace">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj" fmla="val 4653"/>
+          </a:avLst>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -656,7 +677,7 @@
   <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Completed Working with Excel SmartArt
</commit_message>
<xml_diff>
--- a/07 - Inserting Images and Shapes/MonthlyBudget.xlsx
+++ b/07 - Inserting Images and Shapes/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/07 - Inserting Images and Shapes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6218C0B-6658-4A33-B89D-64EF6CECB6B7}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7E3BDC5-E0E6-4C57-AC80-077BA10A2192}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,6 +211,2895 @@
 </styleSheet>
 </file>
 
+<file path=xl/diagrams/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:colorsDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="accent1" pri="11200"/>
+  </dgm:catLst>
+  <dgm:styleLbl name="node0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="lnNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="vennNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgSibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgSibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans1D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="callout">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="conFgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trAlignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidFgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidAlignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidBgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="dkBgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trBgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+        <a:alpha val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="revTx">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="0"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="dk1">
+        <a:alpha val="0"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+</dgm:colorsDef>
+</file>
+
+<file path=xl/diagrams/data1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:dataModel xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <dgm:ptLst>
+    <dgm:pt modelId="{9C67B616-7812-4FCC-AAC4-4D7B59A38CF6}" type="doc">
+      <dgm:prSet loTypeId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3" loCatId="cycle" qsTypeId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1" qsCatId="simple" csTypeId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2" csCatId="accent1" phldr="1"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{2FC42B5E-F2B3-4AE0-8DB5-87B672DBCF02}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t>Make Money</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{3C4116D6-513C-465B-9198-3A484E9D0B0B}" type="parTrans" cxnId="{4FC0B193-3BC4-450A-BC97-9946BE6AB588}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{F2D41A08-2F5F-4324-AA49-54CB1C54262B}" type="sibTrans" cxnId="{4FC0B193-3BC4-450A-BC97-9946BE6AB588}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{F5C7ABDD-63C9-417B-B669-3CE538F4D89C}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t>Spend Money</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{D857C6BE-E72F-4631-8DCA-87BA70E8BC66}" type="parTrans" cxnId="{B3142C96-9A21-4FB4-9799-9141C2E66CA2}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{54F09F84-F2F5-4B27-9DEF-E3ED7A7C0E0C}" type="sibTrans" cxnId="{B3142C96-9A21-4FB4-9799-9141C2E66CA2}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{4B5752BA-98D4-4867-B658-0856D3611015}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t>Track Money</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{BC886E58-6282-4054-AFCD-0EE39F8C179D}" type="parTrans" cxnId="{2E5399FE-2BF0-48E3-B08F-E2C66313858E}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{6324ABBD-7318-4F1B-BB0A-71E47001DC94}" type="sibTrans" cxnId="{2E5399FE-2BF0-48E3-B08F-E2C66313858E}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{9BEB641D-C886-47A1-BDC2-32F45B535616}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t>Work</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{3E3BA56D-44E9-4285-B910-A79076888C62}" type="parTrans" cxnId="{5591E537-2726-4FAA-A488-59554D34303E}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{972C0CD9-68E7-4B8F-8B17-260253BEDF2D}" type="sibTrans" cxnId="{5591E537-2726-4FAA-A488-59554D34303E}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{0CD723C0-0DFD-4EF7-89CA-3002D12C12BC}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t>Ask my Mum</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{F9D17DA4-F022-4ABB-9DA1-BD98D2DDCED1}" type="parTrans" cxnId="{047CB757-2777-4D5D-A28B-2D79B9D6A3BA}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{DE24CA65-4994-43D9-8733-3B01592733A1}" type="sibTrans" cxnId="{047CB757-2777-4D5D-A28B-2D79B9D6A3BA}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{65869761-95FD-4C6F-BAB0-3767021180E6}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t>Bills</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{0B77A85E-B962-4290-86DD-8CDB2E17708F}" type="parTrans" cxnId="{A04E46E0-DEFC-4769-95C6-239E7704FDC6}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{622F1254-AD51-416F-8C84-792F95349A4B}" type="sibTrans" cxnId="{A04E46E0-DEFC-4769-95C6-239E7704FDC6}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{740B2F2B-608A-48B5-9F13-47F324D7C8F1}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t>Movie</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{66DFF24A-D2FA-45A3-808F-4E7A99CE2B21}" type="parTrans" cxnId="{B21B6CC8-0EE1-45A0-8C8F-DD6014AA4E32}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{63F6C266-A26B-4DBB-A0D7-C1A3692C1ADD}" type="sibTrans" cxnId="{B21B6CC8-0EE1-45A0-8C8F-DD6014AA4E32}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{CF4CFE24-0E31-4543-B3A6-669D51D54168}" type="pres">
+      <dgm:prSet presAssocID="{9C67B616-7812-4FCC-AAC4-4D7B59A38CF6}" presName="Name0" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:dir/>
+          <dgm:resizeHandles val="exact"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{D7257417-4858-4E84-ACF3-58F2CBADDD34}" type="pres">
+      <dgm:prSet presAssocID="{9C67B616-7812-4FCC-AAC4-4D7B59A38CF6}" presName="cycle" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{7E6F5A47-C4AA-4CFC-9975-8C0BE852BFD7}" type="pres">
+      <dgm:prSet presAssocID="{2FC42B5E-F2B3-4AE0-8DB5-87B672DBCF02}" presName="nodeFirstNode" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="3">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{EF6FFCEF-3114-4E6C-ACA9-29E8609BE387}" type="pres">
+      <dgm:prSet presAssocID="{F2D41A08-2F5F-4324-AA49-54CB1C54262B}" presName="sibTransFirstNode" presStyleLbl="bgShp" presStyleIdx="0" presStyleCnt="1"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{27F9327D-FF5D-442E-8509-4F2240A0FD3E}" type="pres">
+      <dgm:prSet presAssocID="{F5C7ABDD-63C9-417B-B669-3CE538F4D89C}" presName="nodeFollowingNodes" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="3">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{925A5326-BFD1-4F4F-8989-7A005F690B8F}" type="pres">
+      <dgm:prSet presAssocID="{4B5752BA-98D4-4867-B658-0856D3611015}" presName="nodeFollowingNodes" presStyleLbl="node1" presStyleIdx="2" presStyleCnt="3">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+  </dgm:ptLst>
+  <dgm:cxnLst>
+    <dgm:cxn modelId="{6BCF7C0A-8427-48C7-A57F-B7604A59124B}" type="presOf" srcId="{4B5752BA-98D4-4867-B658-0856D3611015}" destId="{925A5326-BFD1-4F4F-8989-7A005F690B8F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{8F1ECC0F-9358-4498-8434-32FDF03CF7DF}" type="presOf" srcId="{F5C7ABDD-63C9-417B-B669-3CE538F4D89C}" destId="{27F9327D-FF5D-442E-8509-4F2240A0FD3E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{9D5F9D22-7776-4EC6-9074-A9CC95DA6FA7}" type="presOf" srcId="{740B2F2B-608A-48B5-9F13-47F324D7C8F1}" destId="{27F9327D-FF5D-442E-8509-4F2240A0FD3E}" srcOrd="0" destOrd="2" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{9CBC042F-91FD-4295-B2C1-86FFB2B80D09}" type="presOf" srcId="{0CD723C0-0DFD-4EF7-89CA-3002D12C12BC}" destId="{7E6F5A47-C4AA-4CFC-9975-8C0BE852BFD7}" srcOrd="0" destOrd="2" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{5591E537-2726-4FAA-A488-59554D34303E}" srcId="{2FC42B5E-F2B3-4AE0-8DB5-87B672DBCF02}" destId="{9BEB641D-C886-47A1-BDC2-32F45B535616}" srcOrd="0" destOrd="0" parTransId="{3E3BA56D-44E9-4285-B910-A79076888C62}" sibTransId="{972C0CD9-68E7-4B8F-8B17-260253BEDF2D}"/>
+    <dgm:cxn modelId="{91B3BA3B-12AA-40E1-A4FB-A38289FB1139}" type="presOf" srcId="{2FC42B5E-F2B3-4AE0-8DB5-87B672DBCF02}" destId="{7E6F5A47-C4AA-4CFC-9975-8C0BE852BFD7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{23F2D65C-80DA-43F7-8C96-27E4C7D19A0D}" type="presOf" srcId="{F2D41A08-2F5F-4324-AA49-54CB1C54262B}" destId="{EF6FFCEF-3114-4E6C-ACA9-29E8609BE387}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{047CB757-2777-4D5D-A28B-2D79B9D6A3BA}" srcId="{2FC42B5E-F2B3-4AE0-8DB5-87B672DBCF02}" destId="{0CD723C0-0DFD-4EF7-89CA-3002D12C12BC}" srcOrd="1" destOrd="0" parTransId="{F9D17DA4-F022-4ABB-9DA1-BD98D2DDCED1}" sibTransId="{DE24CA65-4994-43D9-8733-3B01592733A1}"/>
+    <dgm:cxn modelId="{5D374E7F-A508-41B7-856F-7FDADAB0F0F8}" type="presOf" srcId="{9C67B616-7812-4FCC-AAC4-4D7B59A38CF6}" destId="{CF4CFE24-0E31-4543-B3A6-669D51D54168}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{4FC0B193-3BC4-450A-BC97-9946BE6AB588}" srcId="{9C67B616-7812-4FCC-AAC4-4D7B59A38CF6}" destId="{2FC42B5E-F2B3-4AE0-8DB5-87B672DBCF02}" srcOrd="0" destOrd="0" parTransId="{3C4116D6-513C-465B-9198-3A484E9D0B0B}" sibTransId="{F2D41A08-2F5F-4324-AA49-54CB1C54262B}"/>
+    <dgm:cxn modelId="{B3142C96-9A21-4FB4-9799-9141C2E66CA2}" srcId="{9C67B616-7812-4FCC-AAC4-4D7B59A38CF6}" destId="{F5C7ABDD-63C9-417B-B669-3CE538F4D89C}" srcOrd="1" destOrd="0" parTransId="{D857C6BE-E72F-4631-8DCA-87BA70E8BC66}" sibTransId="{54F09F84-F2F5-4B27-9DEF-E3ED7A7C0E0C}"/>
+    <dgm:cxn modelId="{68967AAB-ACA5-43E0-9C5E-9D068A0044BB}" type="presOf" srcId="{65869761-95FD-4C6F-BAB0-3767021180E6}" destId="{27F9327D-FF5D-442E-8509-4F2240A0FD3E}" srcOrd="0" destOrd="1" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{B21B6CC8-0EE1-45A0-8C8F-DD6014AA4E32}" srcId="{F5C7ABDD-63C9-417B-B669-3CE538F4D89C}" destId="{740B2F2B-608A-48B5-9F13-47F324D7C8F1}" srcOrd="1" destOrd="0" parTransId="{66DFF24A-D2FA-45A3-808F-4E7A99CE2B21}" sibTransId="{63F6C266-A26B-4DBB-A0D7-C1A3692C1ADD}"/>
+    <dgm:cxn modelId="{119702DF-D5E3-42DA-A80F-31CA5702F1EC}" type="presOf" srcId="{9BEB641D-C886-47A1-BDC2-32F45B535616}" destId="{7E6F5A47-C4AA-4CFC-9975-8C0BE852BFD7}" srcOrd="0" destOrd="1" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{A04E46E0-DEFC-4769-95C6-239E7704FDC6}" srcId="{F5C7ABDD-63C9-417B-B669-3CE538F4D89C}" destId="{65869761-95FD-4C6F-BAB0-3767021180E6}" srcOrd="0" destOrd="0" parTransId="{0B77A85E-B962-4290-86DD-8CDB2E17708F}" sibTransId="{622F1254-AD51-416F-8C84-792F95349A4B}"/>
+    <dgm:cxn modelId="{2E5399FE-2BF0-48E3-B08F-E2C66313858E}" srcId="{9C67B616-7812-4FCC-AAC4-4D7B59A38CF6}" destId="{4B5752BA-98D4-4867-B658-0856D3611015}" srcOrd="2" destOrd="0" parTransId="{BC886E58-6282-4054-AFCD-0EE39F8C179D}" sibTransId="{6324ABBD-7318-4F1B-BB0A-71E47001DC94}"/>
+    <dgm:cxn modelId="{05434024-05E8-48BF-BE61-FEAAD61D265F}" type="presParOf" srcId="{CF4CFE24-0E31-4543-B3A6-669D51D54168}" destId="{D7257417-4858-4E84-ACF3-58F2CBADDD34}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{EFD671E5-AED6-46EC-AFE1-77DBD30E81B0}" type="presParOf" srcId="{D7257417-4858-4E84-ACF3-58F2CBADDD34}" destId="{7E6F5A47-C4AA-4CFC-9975-8C0BE852BFD7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{91BBBB96-3880-47C6-B43E-62510B4948B0}" type="presParOf" srcId="{D7257417-4858-4E84-ACF3-58F2CBADDD34}" destId="{EF6FFCEF-3114-4E6C-ACA9-29E8609BE387}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{E28EDD99-B8E0-4D29-951E-3F3A0EB5D8BE}" type="presParOf" srcId="{D7257417-4858-4E84-ACF3-58F2CBADDD34}" destId="{27F9327D-FF5D-442E-8509-4F2240A0FD3E}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+    <dgm:cxn modelId="{913C6F08-6A3F-493C-BAA0-65F388D9F236}" type="presParOf" srcId="{D7257417-4858-4E84-ACF3-58F2CBADDD34}" destId="{925A5326-BFD1-4F4F-8989-7A005F690B8F}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3"/>
+  </dgm:cxnLst>
+  <dgm:bg/>
+  <dgm:whole/>
+  <dgm:extLst>
+    <a:ext uri="http://schemas.microsoft.com/office/drawing/2008/diagram">
+      <dsp:dataModelExt xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" relId="rId5" minVer="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+    </a:ext>
+  </dgm:extLst>
+</dgm:dataModel>
+</file>
+
+<file path=xl/diagrams/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<dsp:drawing xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <dsp:spTree>
+    <dsp:nvGrpSpPr>
+      <dsp:cNvPr id="0" name=""/>
+      <dsp:cNvGrpSpPr/>
+    </dsp:nvGrpSpPr>
+    <dsp:grpSpPr/>
+    <dsp:sp modelId="{EF6FFCEF-3114-4E6C-ACA9-29E8609BE387}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="911559" y="-127567"/>
+          <a:ext cx="2751602" cy="2751602"/>
+        </a:xfrm>
+        <a:prstGeom prst="circularArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 5689"/>
+            <a:gd name="adj2" fmla="val 340510"/>
+            <a:gd name="adj3" fmla="val 12597188"/>
+            <a:gd name="adj4" fmla="val 18145884"/>
+            <a:gd name="adj5" fmla="val 5908"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:tint val="40000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{7E6F5A47-C4AA-4CFC-9975-8C0BE852BFD7}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="1355886" y="443"/>
+          <a:ext cx="1862947" cy="931473"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="60960" tIns="60960" rIns="60960" bIns="60960" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="711200">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" kern="1200"/>
+            <a:t>Make Money</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="114300" lvl="1" indent="-114300" algn="l" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="15000"/>
+            </a:spcAft>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" kern="1200"/>
+            <a:t>Work</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="114300" lvl="1" indent="-114300" algn="l" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="15000"/>
+            </a:spcAft>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" kern="1200"/>
+            <a:t>Ask my Mum</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="1401357" y="45914"/>
+        <a:ext cx="1772005" cy="840531"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{27F9327D-FF5D-442E-8509-4F2240A0FD3E}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="2398756" y="1806747"/>
+          <a:ext cx="1862947" cy="931473"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="60960" tIns="60960" rIns="60960" bIns="60960" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="711200">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" kern="1200"/>
+            <a:t>Spend Money</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="114300" lvl="1" indent="-114300" algn="l" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="15000"/>
+            </a:spcAft>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" kern="1200"/>
+            <a:t>Bills</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="114300" lvl="1" indent="-114300" algn="l" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="15000"/>
+            </a:spcAft>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1200" kern="1200"/>
+            <a:t>Movie</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="2444227" y="1852218"/>
+        <a:ext cx="1772005" cy="840531"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{925A5326-BFD1-4F4F-8989-7A005F690B8F}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="313016" y="1806747"/>
+          <a:ext cx="1862947" cy="931473"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="60960" tIns="60960" rIns="60960" bIns="60960" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="711200">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" kern="1200"/>
+            <a:t>Track Money</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="358487" y="1852218"/>
+        <a:ext cx="1772005" cy="840531"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+  </dsp:spTree>
+</dsp:drawing>
+</file>
+
+<file path=xl/diagrams/layout1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:layoutDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/layout/cycle3">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="cycle" pri="5000"/>
+  </dgm:catLst>
+  <dgm:sampData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="2">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="3">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="4">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="5">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="6" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="7" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="8" srcId="0" destId="3" srcOrd="2" destOrd="0"/>
+        <dgm:cxn modelId="9" srcId="0" destId="4" srcOrd="3" destOrd="0"/>
+        <dgm:cxn modelId="10" srcId="0" destId="5" srcOrd="4" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:sampData>
+  <dgm:styleData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1"/>
+        <dgm:pt modelId="2"/>
+        <dgm:pt modelId="3"/>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="4" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="5" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="6" srcId="0" destId="3" srcOrd="2" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:styleData>
+  <dgm:clrData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1"/>
+        <dgm:pt modelId="2"/>
+        <dgm:pt modelId="3"/>
+        <dgm:pt modelId="4"/>
+        <dgm:pt modelId="5"/>
+        <dgm:pt modelId="6"/>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="7" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="8" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="9" srcId="0" destId="3" srcOrd="2" destOrd="0"/>
+        <dgm:cxn modelId="10" srcId="0" destId="4" srcOrd="3" destOrd="0"/>
+        <dgm:cxn modelId="11" srcId="0" destId="5" srcOrd="4" destOrd="0"/>
+        <dgm:cxn modelId="12" srcId="0" destId="6" srcOrd="5" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:clrData>
+  <dgm:layoutNode name="Name0">
+    <dgm:varLst>
+      <dgm:dir/>
+      <dgm:resizeHandles val="exact"/>
+    </dgm:varLst>
+    <dgm:choose name="Name1">
+      <dgm:if name="Name2" axis="ch" ptType="node" func="cnt" op="equ" val="2">
+        <dgm:alg type="composite">
+          <dgm:param type="ar" val="0.9"/>
+        </dgm:alg>
+        <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+          <dgm:adjLst/>
+        </dgm:shape>
+        <dgm:presOf/>
+        <dgm:constrLst>
+          <dgm:constr type="primFontSz" for="ch" ptType="node" op="equ" val="65"/>
+          <dgm:constr type="ctrX" for="ch" forName="node1" refType="w" fact="0.5"/>
+          <dgm:constr type="t" for="ch" forName="node1"/>
+          <dgm:constr type="w" for="ch" forName="node1" refType="w" fact="0.8"/>
+          <dgm:constr type="h" for="ch" forName="node1" refType="w" refFor="ch" refForName="node1" fact="0.5"/>
+          <dgm:constr type="ctrX" for="ch" forName="sibTrans" refType="w" fact="0.5"/>
+          <dgm:constr type="t" for="ch" forName="sibTrans"/>
+          <dgm:constr type="w" for="ch" forName="sibTrans" refType="w" fact="0.8"/>
+          <dgm:constr type="h" for="ch" forName="sibTrans" refType="w" refFor="ch" refForName="node1" fact="0.5"/>
+          <dgm:constr type="userA" for="ch" forName="sibTrans" refType="w" fact="1.07"/>
+          <dgm:constr type="ctrX" for="ch" forName="node2" refType="w" fact="0.5"/>
+          <dgm:constr type="b" for="ch" forName="node2" refType="h"/>
+          <dgm:constr type="w" for="ch" forName="node2" refType="w" fact="0.8"/>
+          <dgm:constr type="h" for="ch" forName="node2" refType="w" refFor="ch" refForName="node1" fact="0.5"/>
+          <dgm:constr type="l" for="ch" forName="sp1"/>
+          <dgm:constr type="t" for="ch" forName="sp1" refType="h" fact="0.5"/>
+          <dgm:constr type="w" for="ch" forName="sp1" val="1"/>
+          <dgm:constr type="h" for="ch" forName="sp1" val="1"/>
+          <dgm:constr type="r" for="ch" forName="sp2" refType="w"/>
+          <dgm:constr type="t" for="ch" forName="sp2" refType="h" fact="0.5"/>
+          <dgm:constr type="w" for="ch" forName="sp2" val="1"/>
+          <dgm:constr type="h" for="ch" forName="sp2" val="1"/>
+        </dgm:constrLst>
+        <dgm:ruleLst/>
+      </dgm:if>
+      <dgm:else name="Name3">
+        <dgm:alg type="composite"/>
+        <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+          <dgm:adjLst/>
+        </dgm:shape>
+        <dgm:presOf/>
+        <dgm:constrLst>
+          <dgm:constr type="primFontSz" for="ch" ptType="node" op="equ" val="65"/>
+        </dgm:constrLst>
+        <dgm:ruleLst/>
+      </dgm:else>
+    </dgm:choose>
+    <dgm:choose name="Name4">
+      <dgm:if name="Name5" axis="ch" ptType="node" func="cnt" op="equ" val="2">
+        <dgm:layoutNode name="node1">
+          <dgm:varLst>
+            <dgm:bulletEnabled val="1"/>
+          </dgm:varLst>
+          <dgm:alg type="tx"/>
+          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+            <dgm:adjLst/>
+          </dgm:shape>
+          <dgm:presOf axis="ch desOrSelf" ptType="node node" st="1 1" cnt="1 0"/>
+          <dgm:constrLst>
+            <dgm:constr type="tMarg" refType="primFontSz" fact="0.3"/>
+            <dgm:constr type="bMarg" refType="primFontSz" fact="0.3"/>
+            <dgm:constr type="lMarg" refType="primFontSz" fact="0.3"/>
+            <dgm:constr type="rMarg" refType="primFontSz" fact="0.3"/>
+          </dgm:constrLst>
+          <dgm:ruleLst>
+            <dgm:rule type="primFontSz" val="5" fact="NaN" max="NaN"/>
+          </dgm:ruleLst>
+        </dgm:layoutNode>
+        <dgm:layoutNode name="sibTrans" styleLbl="bgShp">
+          <dgm:choose name="Name6">
+            <dgm:if name="Name7" func="var" arg="dir" op="equ" val="norm">
+              <dgm:alg type="conn">
+                <dgm:param type="connRout" val="longCurve"/>
+                <dgm:param type="begPts" val="midR"/>
+                <dgm:param type="endPts" val="midL"/>
+                <dgm:param type="dstNode" val="node1"/>
+              </dgm:alg>
+              <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="conn" r:blip="" zOrderOff="-2">
+                <dgm:adjLst/>
+              </dgm:shape>
+              <dgm:presOf axis="ch" ptType="sibTrans"/>
+              <dgm:constrLst>
+                <dgm:constr type="userA"/>
+                <dgm:constr type="diam" refType="userA" fact="-1"/>
+                <dgm:constr type="wArH" refType="userA" fact="0.05"/>
+                <dgm:constr type="hArH" refType="userA" fact="0.1"/>
+                <dgm:constr type="stemThick" refType="userA" fact="0.06"/>
+                <dgm:constr type="begPad" refType="connDist" fact="-0.2"/>
+                <dgm:constr type="endPad" refType="connDist" fact="0.05"/>
+              </dgm:constrLst>
+            </dgm:if>
+            <dgm:else name="Name8">
+              <dgm:alg type="conn">
+                <dgm:param type="connRout" val="longCurve"/>
+                <dgm:param type="begPts" val="midL"/>
+                <dgm:param type="endPts" val="midR"/>
+                <dgm:param type="dstNode" val="node1"/>
+              </dgm:alg>
+              <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="conn" r:blip="" zOrderOff="-2">
+                <dgm:adjLst/>
+              </dgm:shape>
+              <dgm:presOf axis="ch" ptType="sibTrans"/>
+              <dgm:constrLst>
+                <dgm:constr type="userA"/>
+                <dgm:constr type="diam" refType="userA"/>
+                <dgm:constr type="wArH" refType="userA" fact="0.05"/>
+                <dgm:constr type="hArH" refType="userA" fact="0.1"/>
+                <dgm:constr type="stemThick" refType="userA" fact="0.06"/>
+                <dgm:constr type="begPad" refType="connDist" fact="-0.2"/>
+                <dgm:constr type="endPad" refType="connDist" fact="0.05"/>
+              </dgm:constrLst>
+            </dgm:else>
+          </dgm:choose>
+          <dgm:ruleLst/>
+        </dgm:layoutNode>
+        <dgm:layoutNode name="node2">
+          <dgm:varLst>
+            <dgm:bulletEnabled val="1"/>
+          </dgm:varLst>
+          <dgm:alg type="tx"/>
+          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+            <dgm:adjLst/>
+          </dgm:shape>
+          <dgm:presOf axis="ch desOrSelf" ptType="node node" st="2 1" cnt="1 0"/>
+          <dgm:constrLst>
+            <dgm:constr type="tMarg" refType="primFontSz" fact="0.3"/>
+            <dgm:constr type="bMarg" refType="primFontSz" fact="0.3"/>
+            <dgm:constr type="lMarg" refType="primFontSz" fact="0.3"/>
+            <dgm:constr type="rMarg" refType="primFontSz" fact="0.3"/>
+          </dgm:constrLst>
+          <dgm:ruleLst>
+            <dgm:rule type="primFontSz" val="5" fact="NaN" max="NaN"/>
+          </dgm:ruleLst>
+        </dgm:layoutNode>
+        <dgm:layoutNode name="sp1">
+          <dgm:alg type="sp"/>
+          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+            <dgm:adjLst/>
+          </dgm:shape>
+          <dgm:presOf/>
+          <dgm:constrLst/>
+          <dgm:ruleLst/>
+        </dgm:layoutNode>
+        <dgm:layoutNode name="sp2">
+          <dgm:alg type="sp"/>
+          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+            <dgm:adjLst/>
+          </dgm:shape>
+          <dgm:presOf/>
+          <dgm:constrLst/>
+          <dgm:ruleLst/>
+        </dgm:layoutNode>
+      </dgm:if>
+      <dgm:else name="Name9">
+        <dgm:layoutNode name="cycle">
+          <dgm:choose name="Name10">
+            <dgm:if name="Name11" func="var" arg="dir" op="equ" val="norm">
+              <dgm:alg type="cycle">
+                <dgm:param type="stAng" val="0"/>
+                <dgm:param type="spanAng" val="360"/>
+              </dgm:alg>
+              <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+                <dgm:adjLst/>
+              </dgm:shape>
+              <dgm:presOf/>
+              <dgm:constrLst>
+                <dgm:constr type="diam" refType="w"/>
+                <dgm:constr type="w" for="ch" ptType="node" refType="w"/>
+                <dgm:constr type="sibSp" val="15"/>
+                <dgm:constr type="userA" for="ch" ptType="sibTrans" refType="diam" op="equ" fact="-1"/>
+                <dgm:constr type="wArH" for="ch" ptType="sibTrans" refType="diam" op="equ" fact="0.05"/>
+                <dgm:constr type="hArH" for="ch" ptType="sibTrans" refType="diam" op="equ" fact="0.1"/>
+                <dgm:constr type="stemThick" for="ch" ptType="sibTrans" refType="diam" op="equ" fact="0.065"/>
+                <dgm:constr type="primFontSz" for="ch" ptType="node" op="equ"/>
+              </dgm:constrLst>
+            </dgm:if>
+            <dgm:else name="Name12">
+              <dgm:alg type="cycle">
+                <dgm:param type="stAng" val="0"/>
+                <dgm:param type="spanAng" val="-360"/>
+              </dgm:alg>
+              <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+                <dgm:adjLst/>
+              </dgm:shape>
+              <dgm:presOf/>
+              <dgm:constrLst>
+                <dgm:constr type="diam" refType="w"/>
+                <dgm:constr type="w" for="ch" ptType="node" refType="w"/>
+                <dgm:constr type="sibSp" val="15"/>
+                <dgm:constr type="userA" for="ch" ptType="sibTrans" refType="diam" op="equ"/>
+                <dgm:constr type="wArH" for="ch" ptType="sibTrans" refType="diam" op="equ" fact="0.05"/>
+                <dgm:constr type="hArH" for="ch" ptType="sibTrans" refType="diam" op="equ" fact="0.1"/>
+                <dgm:constr type="stemThick" for="ch" ptType="sibTrans" refType="diam" op="equ" fact="0.065"/>
+                <dgm:constr type="primFontSz" for="ch" ptType="node" op="equ"/>
+              </dgm:constrLst>
+            </dgm:else>
+          </dgm:choose>
+          <dgm:ruleLst/>
+          <dgm:forEach name="nodesFirstNodeForEach" axis="ch" ptType="node" cnt="1">
+            <dgm:layoutNode name="nodeFirstNode">
+              <dgm:varLst>
+                <dgm:bulletEnabled val="1"/>
+              </dgm:varLst>
+              <dgm:alg type="tx"/>
+              <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+                <dgm:adjLst/>
+              </dgm:shape>
+              <dgm:presOf axis="desOrSelf" ptType="node"/>
+              <dgm:constrLst>
+                <dgm:constr type="h" refType="w" fact="0.5"/>
+                <dgm:constr type="primFontSz" val="65"/>
+                <dgm:constr type="tMarg" refType="primFontSz" fact="0.3"/>
+                <dgm:constr type="bMarg" refType="primFontSz" fact="0.3"/>
+                <dgm:constr type="lMarg" refType="primFontSz" fact="0.3"/>
+                <dgm:constr type="rMarg" refType="primFontSz" fact="0.3"/>
+              </dgm:constrLst>
+              <dgm:ruleLst>
+                <dgm:rule type="primFontSz" val="5" fact="NaN" max="NaN"/>
+              </dgm:ruleLst>
+            </dgm:layoutNode>
+            <dgm:forEach name="sibTransForEach" axis="followSib" ptType="sibTrans" cnt="1">
+              <dgm:layoutNode name="sibTransFirstNode" styleLbl="bgShp">
+                <dgm:choose name="Name13">
+                  <dgm:if name="Name14" func="var" arg="dir" op="equ" val="norm">
+                    <dgm:alg type="conn">
+                      <dgm:param type="connRout" val="longCurve"/>
+                      <dgm:param type="begPts" val="midR"/>
+                      <dgm:param type="endPts" val="midL"/>
+                      <dgm:param type="dstNode" val="nodeFirstNode"/>
+                    </dgm:alg>
+                  </dgm:if>
+                  <dgm:else name="Name15">
+                    <dgm:alg type="conn">
+                      <dgm:param type="connRout" val="longCurve"/>
+                      <dgm:param type="begPts" val="midL"/>
+                      <dgm:param type="endPts" val="midR"/>
+                      <dgm:param type="dstNode" val="nodeFirstNode"/>
+                    </dgm:alg>
+                  </dgm:else>
+                </dgm:choose>
+                <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="conn" r:blip="" zOrderOff="-2">
+                  <dgm:adjLst/>
+                </dgm:shape>
+                <dgm:presOf axis="self"/>
+                <dgm:choose name="Name16">
+                  <dgm:if name="Name17" axis="par ch" ptType="doc node" func="cnt" op="equ" val="3">
+                    <dgm:constrLst>
+                      <dgm:constr type="userA"/>
+                      <dgm:constr type="diam" refType="userA" fact="1.01"/>
+                      <dgm:constr type="begPad" refType="connDist" fact="-0.2"/>
+                      <dgm:constr type="endPad" refType="connDist" fact="0.05"/>
+                    </dgm:constrLst>
+                  </dgm:if>
+                  <dgm:if name="Name18" axis="par ch" ptType="doc node" func="cnt" op="equ" val="4">
+                    <dgm:constrLst>
+                      <dgm:constr type="userA"/>
+                      <dgm:constr type="diam" refType="userA" fact="1.26"/>
+                      <dgm:constr type="begPad" refType="connDist" fact="-0.2"/>
+                      <dgm:constr type="endPad" refType="connDist" fact="0.05"/>
+                    </dgm:constrLst>
+                  </dgm:if>
+                  <dgm:if name="Name19" axis="par ch" ptType="doc node" func="cnt" op="equ" val="5">
+                    <dgm:constrLst>
+                      <dgm:constr type="userA"/>
+                      <dgm:constr type="diam" refType="userA" fact="1.04"/>
+                      <dgm:constr type="begPad" refType="connDist" fact="-0.2"/>
+                      <dgm:constr type="endPad" refType="connDist" fact="0.05"/>
+                    </dgm:constrLst>
+                  </dgm:if>
+                  <dgm:if name="Name20" axis="par ch" ptType="doc node" func="cnt" op="equ" val="6">
+                    <dgm:constrLst>
+                      <dgm:constr type="userA"/>
+                      <dgm:constr type="diam" refType="userA" fact="1.1"/>
+                      <dgm:constr type="begPad" refType="connDist" fact="-0.2"/>
+                      <dgm:constr type="endPad" refType="connDist" fact="0.05"/>
+                    </dgm:constrLst>
+                  </dgm:if>
+                  <dgm:else name="Name21">
+                    <dgm:constrLst>
+                      <dgm:constr type="userA"/>
+                      <dgm:constr type="diam" refType="userA" fact="1.04"/>
+                      <dgm:constr type="begPad" refType="connDist" fact="-0.2"/>
+                      <dgm:constr type="endPad" refType="connDist" fact="0.05"/>
+                    </dgm:constrLst>
+                  </dgm:else>
+                </dgm:choose>
+                <dgm:ruleLst/>
+              </dgm:layoutNode>
+            </dgm:forEach>
+          </dgm:forEach>
+          <dgm:forEach name="followingNodesForEach" axis="ch" ptType="node" st="2">
+            <dgm:layoutNode name="nodeFollowingNodes">
+              <dgm:varLst>
+                <dgm:bulletEnabled val="1"/>
+              </dgm:varLst>
+              <dgm:alg type="tx"/>
+              <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+                <dgm:adjLst/>
+              </dgm:shape>
+              <dgm:presOf axis="desOrSelf" ptType="node"/>
+              <dgm:constrLst>
+                <dgm:constr type="h" refType="w" fact="0.5"/>
+                <dgm:constr type="primFontSz" val="65"/>
+                <dgm:constr type="tMarg" refType="primFontSz" fact="0.3"/>
+                <dgm:constr type="bMarg" refType="primFontSz" fact="0.3"/>
+                <dgm:constr type="lMarg" refType="primFontSz" fact="0.3"/>
+                <dgm:constr type="rMarg" refType="primFontSz" fact="0.3"/>
+              </dgm:constrLst>
+              <dgm:ruleLst>
+                <dgm:rule type="primFontSz" val="5" fact="NaN" max="NaN"/>
+              </dgm:ruleLst>
+            </dgm:layoutNode>
+          </dgm:forEach>
+        </dgm:layoutNode>
+      </dgm:else>
+    </dgm:choose>
+  </dgm:layoutNode>
+</dgm:layoutDef>
+</file>
+
+<file path=xl/diagrams/quickStyle1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:styleDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="simple" pri="10100"/>
+  </dgm:catLst>
+  <dgm:scene3d>
+    <a:camera prst="orthographicFront"/>
+    <a:lightRig rig="threePt" dir="t"/>
+  </dgm:scene3d>
+  <dgm:styleLbl name="node0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="lnNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="vennNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="tx1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgSibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgSibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans1D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="callout">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="conFgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trAlignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidFgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidAlignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidBgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="dkBgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trBgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="revTx">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+</dgm:styleDef>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -352,6 +3241,42 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>307521</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>111578</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>103413</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>74385</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagram 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{675AE01E-7FAE-96DF-F016-9900484EBF07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+          <dgm:relIds xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:dm="rId1" r:lo="rId2" r:qs="rId3" r:cs="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -676,8 +3601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>